<commit_message>
updated investigation view design and todo list
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>ToDo:</t>
   </si>
@@ -45,6 +45,51 @@
   </si>
   <si>
     <t>prescription and navigation not working well</t>
+  </si>
+  <si>
+    <t>Assigned</t>
+  </si>
+  <si>
+    <t>Sharmila</t>
+  </si>
+  <si>
+    <t>Onhold</t>
+  </si>
+  <si>
+    <t>OnHold</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Taniya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User need to click on Print
+ button at many times to print prescription E.g. Click on button "PrintPrescription" then click on Print then click on print. We should allow user to click only once to print prescription      </t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>Grid
+ or popup should display on clinical examination and Investigation .e.g . If patient came 4 times as OPD so user should able to see patient BP values according to OPD Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user cannot scroll year in dob control </t>
+  </si>
+  <si>
+    <t>add patient  form needs to design properly</t>
+  </si>
+  <si>
+    <t>add new patient if patient is female spouse should get 
+updated as male</t>
+  </si>
+  <si>
+    <t>upload file button look needs to change</t>
+  </si>
+  <si>
+    <t>automatic logoff should get removed and add button for logoff</t>
   </si>
 </sst>
 </file>
@@ -80,8 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,19 +410,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -384,37 +432,162 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit for the Small defecs as per todo list.
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\HospitalManagement30Dec\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>ToDo:</t>
   </si>
@@ -93,12 +88,27 @@
   </si>
   <si>
     <t>Add one more column in prescription intake adv (medicine should take after food / before food / not appplicable/ in morning immidietly after get up/ In night before bed)</t>
+  </si>
+  <si>
+    <t>Please change the backgroud color.</t>
+  </si>
+  <si>
+    <t>Once session timeout it gets log off. I update the session timeout after 30min from ideal. If its still not working please let me know.</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Default save message should get removed.</t>
+  </si>
+  <si>
+    <t>Submit button and Button style should same</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -193,7 +203,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -228,7 +238,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -405,7 +415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -413,19 +423,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -438,8 +449,11 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -453,7 +467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -467,7 +481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -481,7 +495,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -495,7 +509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -503,13 +517,13 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -523,7 +537,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -531,13 +545,13 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -545,13 +559,13 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -565,7 +579,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -579,7 +593,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -587,13 +601,16 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -604,6 +621,48 @@
         <v>14</v>
       </c>
       <c r="D13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commi for Updated ToDoList. There is no any pending task for me(Taniya).
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -415,7 +415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +531,7 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -618,7 +618,7 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>

</xml_diff>